<commit_message>
Update test file with empty cells
</commit_message>
<xml_diff>
--- a/test_data/test_1.xlsx
+++ b/test_data/test_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBEC798-F372-8F48-B813-CB900CEDAC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4493EE52-2D80-4840-A99C-8F5797D1CBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68320" yWindow="2520" windowWidth="33260" windowHeight="19480" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="1200" yWindow="500" windowWidth="33260" windowHeight="19480" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="256">
   <si>
     <t>Epoch</t>
   </si>
@@ -951,10 +951,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1965,7 +1965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679CED36-1B68-6F40-B862-B156999A55CA}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:E2"/>
     </sheetView>
   </sheetViews>
@@ -1980,34 +1980,34 @@
       <c r="A1" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>253</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>252</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
@@ -2035,54 +2035,54 @@
       <c r="A6" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
@@ -2149,16 +2149,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2168,11 +2168,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2221,9 +2221,7 @@
       <c r="D2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
         <v>24</v>
       </c>
@@ -2247,9 +2245,7 @@
       <c r="D3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
         <v>24</v>
       </c>
@@ -2269,9 +2265,7 @@
       <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
         <v>24</v>
       </c>
@@ -2291,9 +2285,7 @@
       <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
         <v>24</v>
       </c>
@@ -2389,15 +2381,9 @@
       <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
         <v>24</v>
       </c>
@@ -2409,9 +2395,7 @@
       <c r="B11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="C11" s="4"/>
       <c r="D11" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Updates using new USDM version
</commit_message>
<xml_diff>
--- a/test_data/test_1.xlsx
+++ b/test_data/test_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A712EF-C25C-814E-B916-F4AB62AFC146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11A2CAE-7D6C-2044-894A-DB2C9A838260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="500" windowWidth="33260" windowHeight="19480" activeTab="8" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="340" yWindow="500" windowWidth="33260" windowHeight="19480" firstSheet="1" activeTab="11" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="265">
   <si>
     <t>Epoch</t>
   </si>
@@ -833,6 +833,15 @@
   </si>
   <si>
     <t>Test Nine</t>
+  </si>
+  <si>
+    <t>SDR Prev Next</t>
+  </si>
+  <si>
+    <t>SDR</t>
+  </si>
+  <si>
+    <t>SDR Root</t>
   </si>
 </sst>
 </file>
@@ -972,10 +981,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1865,14 +1874,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1890,6 +1900,22 @@
       </c>
       <c r="B2" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2020,34 +2046,34 @@
       <c r="A3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="27" t="s">
         <v>163</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
@@ -2167,16 +2193,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3145,7 +3171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D608A778-255D-4443-A7EA-03049F1FC98F}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>